<commit_message>
Initial commit for V2.0 HW
HW completed
Layout completed
Tasks updated
</commit_message>
<xml_diff>
--- a/hardware/wakeuplight rev1/Mistakes and notes.xlsx
+++ b/hardware/wakeuplight rev1/Mistakes and notes.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -39,15 +39,6 @@
     <t>Corrected in Rev2?</t>
   </si>
   <si>
-    <t>Footprint</t>
-  </si>
-  <si>
-    <t>CSD88539ND is a NFET. Currently connected as PFET</t>
-  </si>
-  <si>
-    <t>Body diode will cause the transistor to be always ON</t>
-  </si>
-  <si>
     <t>Yes, changed NFET wiring</t>
   </si>
   <si>
@@ -139,6 +130,33 @@
   </si>
   <si>
     <t>Critical</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Sticking with this fet, SO-8 is very common, can be substituted for cheaper fet</t>
+  </si>
+  <si>
+    <t>Add thermal pads under FETs</t>
+  </si>
+  <si>
+    <t>Fets get very hot, used for thermal releif</t>
+  </si>
+  <si>
+    <t>Not required, as it would still operate within specs, though, better ventilation might help</t>
+  </si>
+  <si>
+    <t>Requires complete re-layout, so not going to do it this version, maybe in future versions</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Top left is pin 1, easily recognizable. No action</t>
   </si>
 </sst>
 </file>
@@ -154,12 +172,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -174,12 +198,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,16 +526,18 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -529,55 +560,64 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>42469</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>42469</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>42469</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>17</v>
+      <c r="F4" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -594,129 +634,150 @@
         <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>42469</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="F6" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>42469</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>42469</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>42469</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="5" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>42469</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="E10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="1" t="s">
+      <c r="F10" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>42469</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
-        <v>42469</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>42469</v>
+        <v>42476</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>